<commit_message>
Added data new banks and updated manusript
</commit_message>
<xml_diff>
--- a/data/DBbanks/CAR_IRR_3A6_missing.xlsx
+++ b/data/DBbanks/CAR_IRR_3A6_missing.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9bf72e6496f26e8d/UWA PhD/bankFailure/data/DBbanks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_F918B675C3574AFC124848D4024E49F8213371BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9706BD4-E2B3-45E0-BFA8-41C6EAB570F7}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_F918B675C3574AFC124848D4024E49F8213371BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD2523F2-1420-455F-B200-2E7F08C36EB2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12396" yWindow="-108" windowWidth="12504" windowHeight="9432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Missing2000q4" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$287</definedName>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="70">
   <si>
     <t>IDENT</t>
   </si>
@@ -226,15 +228,31 @@
   <si>
     <t>esd_1997-04_1998-07_long_f3fecha</t>
   </si>
+  <si>
+    <t>2001q2</t>
+  </si>
+  <si>
+    <t>2001q1</t>
+  </si>
+  <si>
+    <t>2000q4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,14 +275,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{D6BD3370-36B6-4221-818B-24074D4D6EF8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -578,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K287"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -10643,7 +10664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86876851-6F2F-4276-8259-D2AB327B3B35}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -11256,4 +11277,170 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290E2B95-E8D4-422F-9F12-52553950ACA1}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
+        <v>94</v>
+      </c>
+      <c r="C5" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
+        <v>97</v>
+      </c>
+      <c r="C6" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <v>301</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
+        <v>44059</v>
+      </c>
+      <c r="C8" s="1">
+        <v>83</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
+        <v>64123</v>
+      </c>
+      <c r="C9" s="1">
+        <v>94</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10" s="1">
+        <v>97</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C11" s="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12" s="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13" s="1">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C14" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C15" s="1">
+        <v>303</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C16" s="1">
+        <v>44059</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F25B15-1732-428D-B147-6E8C986F09AF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>